<commit_message>
Aggiunto sender per Microsoft Exchange
</commit_message>
<xml_diff>
--- a/running_job.xlsx
+++ b/running_job.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Nome del report</t>
   </si>
@@ -37,13 +37,16 @@
     <t>Report estrazione data</t>
   </si>
   <si>
+    <t>00 46 09 ? * MON,TUE,WED,THU,FRI</t>
+  </si>
+  <si>
+    <t>NO-RUNS</t>
+  </si>
+  <si>
+    <t>report2</t>
+  </si>
+  <si>
     <t>00 31 12 ? * MON,TUE,WED,THU,FRI</t>
-  </si>
-  <si>
-    <t>NO-RUNS</t>
-  </si>
-  <si>
-    <t>report2</t>
   </si>
   <si>
     <t>Nome DataSource</t>
@@ -252,7 +255,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="2">
         <v>8</v>
@@ -280,18 +283,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -312,17 +315,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inizio del servizio rest per la modifica dei report schedulati
</commit_message>
<xml_diff>
--- a/running_job.xlsx
+++ b/running_job.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Nome del report</t>
   </si>
@@ -31,34 +31,28 @@
     <t>Data fine ultima Esecuzione</t>
   </si>
   <si>
-    <t>report1</t>
+    <t>report2</t>
   </si>
   <si>
     <t>Report estrazione data</t>
   </si>
   <si>
-    <t>00 46 09 ? * MON,TUE,WED,THU,FRI</t>
+    <t>00 31 12 ? * MON,TUE,WED,THU,FRI</t>
   </si>
   <si>
     <t>NO-RUNS</t>
   </si>
   <si>
-    <t>report2</t>
-  </si>
-  <si>
-    <t>00 31 12 ? * MON,TUE,WED,THU,FRI</t>
-  </si>
-  <si>
     <t>Nome DataSource</t>
   </si>
   <si>
     <t>Descrizione DataSource</t>
   </si>
   <si>
-    <t>monet</t>
-  </si>
-  <si>
-    <t>Datasource di sviluppo schema MONET</t>
+    <t>postgres</t>
+  </si>
+  <si>
+    <t>Datasource di produzione schema MONET</t>
   </si>
   <si>
     <t>Nome Template</t>
@@ -200,7 +194,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -247,23 +241,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="2">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -278,23 +255,23 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="17.28125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="36.1015625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="38.7890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -315,17 +292,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunto servizio per lanciare in maniera manuale un report
</commit_message>
<xml_diff>
--- a/running_job.xlsx
+++ b/running_job.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Nome del report</t>
   </si>
@@ -40,7 +40,10 @@
     <t>00 31 12 ? * MON,TUE,WED,THU,FRI</t>
   </si>
   <si>
-    <t>NO-RUNS</t>
+    <t>10/10/2017 22:00:55</t>
+  </si>
+  <si>
+    <t>10/10/2017 22:02:21</t>
   </si>
   <si>
     <t>Nome DataSource</t>
@@ -238,7 +241,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -260,18 +263,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -292,17 +295,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunto servizio per recupero dettaglio datasources
</commit_message>
<xml_diff>
--- a/running_job.xlsx
+++ b/running_job.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Nome del report</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>NO-RUNS</t>
+  </si>
+  <si>
+    <t>report2</t>
+  </si>
+  <si>
+    <t>00 00 10 ? * MON,TUE,WED,THU,FRI</t>
   </si>
   <si>
     <t>Nome DataSource</t>
@@ -194,7 +200,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -241,6 +247,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -260,18 +283,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -292,17 +315,17 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>